<commit_message>
Pour publication release 4.0.4 0f95c4b0d67b264a89aa0d25526b71c931aa165d
</commit_message>
<xml_diff>
--- a/Publication-release-404/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/Publication-release-404/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.3</t>
+    <t>4.0.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-16T14:02:22+00:00</t>
+    <t>2025-06-16T15:13:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>